<commit_message>
ATPG - boligbygging og jernbanetall
</commit_message>
<xml_diff>
--- a/Data/Mobilitet_i_Telemark/Jernbane/Passasjerer/Jernbanestatistikk_2012_2024.xlsx
+++ b/Data/Mobilitet_i_Telemark/Jernbane/Passasjerer/Jernbanestatistikk_2012_2024.xlsx
@@ -1,26 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vestfoldfylke-my.sharepoint.com/personal/rasmus_palmqvist_vestfoldfylke_no/Documents/Dokumenter/Bypakke Vestfoldbyene/Buss CSV_text/Vestfold/Brukes2024/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://telemarkfylke-my.sharepoint.com/personal/kjell-tore_haustveit_telemarkfylke_no/Documents/GitHub/Telemark/Data/Mobilitet_i_Telemark/Jernbane/Passasjerer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="487" documentId="8_{97E84CCC-6234-465C-AE6C-762AAC589669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF60F7B2-E70C-40B1-9866-489448EC8B6A}"/>
+  <xr:revisionPtr revIDLastSave="505" documentId="8_{97E84CCC-6234-465C-AE6C-762AAC589669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{801A58D4-AB1E-4E67-9884-83F13008E355}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="57840" windowHeight="15720" activeTab="1" xr2:uid="{DD3C63B0-74E3-455B-9E64-045F09D85D0E}"/>
+    <workbookView minimized="1" xWindow="312" yWindow="312" windowWidth="21792" windowHeight="15648" activeTab="1" xr2:uid="{DD3C63B0-74E3-455B-9E64-045F09D85D0E}"/>
   </bookViews>
   <sheets>
-    <sheet name="2012-2023" sheetId="1" r:id="rId1"/>
-    <sheet name="2023_2024" sheetId="3" r:id="rId2"/>
-    <sheet name="Tall tatt vekk" sheetId="4" r:id="rId3"/>
+    <sheet name="Ark1" sheetId="5" r:id="rId1"/>
+    <sheet name="2012-2023" sheetId="1" r:id="rId2"/>
+    <sheet name="Ark2" sheetId="6" r:id="rId3"/>
+    <sheet name="2023_2024" sheetId="3" r:id="rId4"/>
+    <sheet name="Tall tatt vekk" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2023_2024'!$A$1:$F$121</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2012-2023'!$A$1:$E$121</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'2023_2024'!$A$1:$F$121</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <pivotCaches>
+    <pivotCache cacheId="4" r:id="rId6"/>
+    <pivotCache cacheId="9" r:id="rId7"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="78">
   <si>
     <t>Togprodukt</t>
   </si>
@@ -252,6 +259,30 @@
   <si>
     <t>Torp stasjon</t>
   </si>
+  <si>
+    <t>Radetiketter</t>
+  </si>
+  <si>
+    <t>Totalsum</t>
+  </si>
+  <si>
+    <t>Summer av Antall_av_på</t>
+  </si>
+  <si>
+    <t>Kolonneetiketter</t>
+  </si>
+  <si>
+    <t>Summer av Påstigninger</t>
+  </si>
+  <si>
+    <t>Totalt Summer av Påstigninger</t>
+  </si>
+  <si>
+    <t>Totalt Summer av Avstigninger</t>
+  </si>
+  <si>
+    <t>Summer av Avstigninger</t>
+  </si>
 </sst>
 </file>
 
@@ -280,6 +311,7 @@
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -343,7 +375,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
@@ -362,6 +394,11 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Komma" xfId="1" builtinId="3"/>
@@ -461,10 +498,2365 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Kjell-Tore Haustveit" refreshedDate="45954.436769907406" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="121" xr:uid="{6F1CA056-9204-4F48-8F04-099D6898B48D}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:D1048576" sheet="2012-2023"/>
+  </cacheSource>
+  <cacheFields count="4">
+    <cacheField name="Togprodukt" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Stasjonsnavn" numFmtId="0">
+      <sharedItems containsBlank="1" count="11">
+        <s v="Holmestrand"/>
+        <s v="Larvik"/>
+        <s v="Porsgrunn"/>
+        <s v="Sande"/>
+        <s v="Sandefjord"/>
+        <s v="Skien"/>
+        <s v="Skoppum"/>
+        <s v="Stokke"/>
+        <s v="Torp"/>
+        <s v="Tønsberg"/>
+        <m/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Antall_av_på" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="67015" maxValue="1464748"/>
+    </cacheField>
+    <cacheField name="År" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="2012" maxValue="2023" count="13">
+        <n v="2012"/>
+        <n v="2013"/>
+        <n v="2014"/>
+        <n v="2015"/>
+        <n v="2016"/>
+        <n v="2017"/>
+        <n v="2018"/>
+        <n v="2019"/>
+        <n v="2020"/>
+        <n v="2021"/>
+        <n v="2022"/>
+        <n v="2023"/>
+        <m/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Kjell-Tore Haustveit" refreshedDate="45954.437604398147" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="161" xr:uid="{3353D399-B111-439D-873F-A1CF1571B90B}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:F1048576" sheet="2023_2024"/>
+  </cacheSource>
+  <cacheFields count="6">
+    <cacheField name="År" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="2023" maxValue="2024" count="3">
+        <n v="2023"/>
+        <n v="2024"/>
+        <m/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Måned_nr" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Måned" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Stasjonsnavn" numFmtId="0">
+      <sharedItems containsBlank="1" count="21">
+        <s v="Holmestrand  "/>
+        <s v="Larvik  "/>
+        <s v="Porsgrunn  "/>
+        <s v="Sande  "/>
+        <s v="Sandefjord  "/>
+        <s v="Skien  "/>
+        <s v="Skoppum  "/>
+        <s v="Stokke  "/>
+        <s v="Torp  "/>
+        <s v="Tønsberg  "/>
+        <s v="Holmestrand stasjon"/>
+        <s v="Larvik stasjon"/>
+        <s v="Porsgrunn stasjon"/>
+        <s v="Sande stasjon"/>
+        <s v="Sandefjord stasjon"/>
+        <s v="Skien stasjon"/>
+        <s v="Skoppum stasjon"/>
+        <s v="Stokke stasjon"/>
+        <s v="Tønsberg stasjon"/>
+        <s v="Torp stasjon"/>
+        <m/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Påstigninger" numFmtId="164">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="5456.6630000000032" maxValue="56888.356000000043"/>
+    </cacheField>
+    <cacheField name="Avstigninger" numFmtId="164">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="5183.4159999999956" maxValue="56953.466999999997"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="121">
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="0"/>
+    <n v="314525"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="1"/>
+    <n v="304197"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="2"/>
+    <n v="141379"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="3"/>
+    <n v="194755"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="4"/>
+    <n v="434447"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="5"/>
+    <n v="80101"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="6"/>
+    <n v="200669"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="7"/>
+    <n v="109481"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="8"/>
+    <n v="113162"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="9"/>
+    <n v="931728"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="0"/>
+    <n v="353599"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="1"/>
+    <n v="321290"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="2"/>
+    <n v="190114"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="3"/>
+    <n v="186446"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="4"/>
+    <n v="469650"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="5"/>
+    <n v="112886"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="6"/>
+    <n v="239920"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="7"/>
+    <n v="116768"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="8"/>
+    <n v="140340"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="9"/>
+    <n v="1042193"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="0"/>
+    <n v="359195"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="1"/>
+    <n v="327977"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="2"/>
+    <n v="198514"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="3"/>
+    <n v="195675"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="4"/>
+    <n v="476502"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="5"/>
+    <n v="119997"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="6"/>
+    <n v="251589"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="7"/>
+    <n v="123843"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="8"/>
+    <n v="143266"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="9"/>
+    <n v="1086214"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="0"/>
+    <n v="379205"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="1"/>
+    <n v="331198"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="2"/>
+    <n v="217635"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="3"/>
+    <n v="209684"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="4"/>
+    <n v="523077"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="5"/>
+    <n v="126139"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="6"/>
+    <n v="281275"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="7"/>
+    <n v="139646"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="8"/>
+    <n v="138141"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="9"/>
+    <n v="1165629"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="0"/>
+    <n v="445746"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="1"/>
+    <n v="399416"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="2"/>
+    <n v="268098"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="3"/>
+    <n v="257728"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="4"/>
+    <n v="650596"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="5"/>
+    <n v="145151"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="6"/>
+    <n v="349818"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="7"/>
+    <n v="179477"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="8"/>
+    <n v="166417"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="9"/>
+    <n v="1464748"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="0"/>
+    <n v="363920"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="1"/>
+    <n v="492976"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="2"/>
+    <n v="95402"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="3"/>
+    <n v="208064"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="4"/>
+    <n v="528753"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="5"/>
+    <n v="77829"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="6"/>
+    <n v="265829"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="7"/>
+    <n v="145204"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="8"/>
+    <n v="159607"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="9"/>
+    <n v="1176354"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="0"/>
+    <n v="354378"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="1"/>
+    <n v="387448"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="2"/>
+    <n v="115993"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="3"/>
+    <n v="213193"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="4"/>
+    <n v="573324"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="5"/>
+    <n v="97152"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="6"/>
+    <n v="269212"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="7"/>
+    <n v="148426"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="8"/>
+    <n v="167068"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="9"/>
+    <n v="1173778"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="0"/>
+    <n v="378078"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="1"/>
+    <n v="396320"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="2"/>
+    <n v="291603"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="3"/>
+    <n v="243057"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="4"/>
+    <n v="615512"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="5"/>
+    <n v="220938"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="6"/>
+    <n v="302231"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="7"/>
+    <n v="161621"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="8"/>
+    <n v="195439"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="9"/>
+    <n v="1314385"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="0"/>
+    <n v="203272"/>
+    <x v="8"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="1"/>
+    <n v="226735"/>
+    <x v="8"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="2"/>
+    <n v="179134"/>
+    <x v="8"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="3"/>
+    <n v="132978"/>
+    <x v="8"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="4"/>
+    <n v="342489"/>
+    <x v="8"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="5"/>
+    <n v="151023"/>
+    <x v="8"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="6"/>
+    <n v="148262"/>
+    <x v="8"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="7"/>
+    <n v="94565"/>
+    <x v="8"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="8"/>
+    <n v="81050"/>
+    <x v="8"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="9"/>
+    <n v="698842"/>
+    <x v="8"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="0"/>
+    <n v="209977"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="1"/>
+    <n v="182074"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="2"/>
+    <n v="151838"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="3"/>
+    <n v="146097"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="4"/>
+    <n v="270316"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="5"/>
+    <n v="127373"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="6"/>
+    <n v="145517"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="7"/>
+    <n v="83301"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="8"/>
+    <n v="67015"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="9"/>
+    <n v="742001"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="0"/>
+    <n v="323386"/>
+    <x v="10"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="1"/>
+    <n v="328021"/>
+    <x v="10"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="2"/>
+    <n v="300022"/>
+    <x v="10"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="3"/>
+    <n v="290272"/>
+    <x v="10"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="4"/>
+    <n v="483295"/>
+    <x v="10"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="5"/>
+    <n v="207067"/>
+    <x v="10"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="6"/>
+    <n v="241594"/>
+    <x v="10"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="7"/>
+    <n v="135171"/>
+    <x v="10"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="8"/>
+    <n v="210024"/>
+    <x v="10"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="9"/>
+    <n v="1086156"/>
+    <x v="10"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="0"/>
+    <n v="383403"/>
+    <x v="11"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="1"/>
+    <n v="424403"/>
+    <x v="11"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="2"/>
+    <n v="454512"/>
+    <x v="11"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="3"/>
+    <n v="275695"/>
+    <x v="11"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="4"/>
+    <n v="638979"/>
+    <x v="11"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="5"/>
+    <n v="362417"/>
+    <x v="11"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="6"/>
+    <n v="303505"/>
+    <x v="11"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="7"/>
+    <n v="211644"/>
+    <x v="11"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="8"/>
+    <n v="224883"/>
+    <x v="11"/>
+  </r>
+  <r>
+    <s v="Eidsvoll - Skien"/>
+    <x v="9"/>
+    <n v="1197623"/>
+    <x v="11"/>
+  </r>
+  <r>
+    <m/>
+    <x v="10"/>
+    <m/>
+    <x v="12"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="161">
+  <r>
+    <x v="0"/>
+    <s v="01"/>
+    <s v="januar"/>
+    <x v="0"/>
+    <n v="17280.326999999994"/>
+    <n v="17052.775000000009"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="02"/>
+    <s v="februar"/>
+    <x v="0"/>
+    <n v="15280.967000000015"/>
+    <n v="15479.641999999993"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="03"/>
+    <s v="mars"/>
+    <x v="0"/>
+    <n v="18573.163"/>
+    <n v="18854.499000000014"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="04"/>
+    <s v="april"/>
+    <x v="0"/>
+    <n v="15432.053999999995"/>
+    <n v="16274.001000000004"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="05"/>
+    <s v="mai"/>
+    <x v="0"/>
+    <n v="16977.195999999996"/>
+    <n v="16668.650000000005"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="06"/>
+    <s v="juni"/>
+    <x v="0"/>
+    <n v="15987.004999999999"/>
+    <n v="16129.301000000001"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="07"/>
+    <s v="juli"/>
+    <x v="0"/>
+    <n v="9533.3749999999927"/>
+    <n v="6513.1080000000102"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="08"/>
+    <s v="august"/>
+    <x v="0"/>
+    <n v="14941.929000000006"/>
+    <n v="14751.840999999999"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="09"/>
+    <s v="september"/>
+    <x v="0"/>
+    <n v="17006.504999999997"/>
+    <n v="16739.808999999997"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="10"/>
+    <s v="oktober"/>
+    <x v="0"/>
+    <n v="17482.546999999999"/>
+    <n v="18180.679"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="11"/>
+    <s v="november"/>
+    <x v="0"/>
+    <n v="18063.820000000003"/>
+    <n v="17970.437000000002"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="12"/>
+    <s v="desember"/>
+    <x v="0"/>
+    <n v="15300.660000000018"/>
+    <n v="16929.951000000015"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="01"/>
+    <s v="januar"/>
+    <x v="1"/>
+    <n v="17521.714999999993"/>
+    <n v="16927.078999999983"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="02"/>
+    <s v="februar"/>
+    <x v="1"/>
+    <n v="15806.699999999995"/>
+    <n v="16191.175999999998"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="03"/>
+    <s v="mars"/>
+    <x v="1"/>
+    <n v="18890.385999999995"/>
+    <n v="18848.862000000026"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="04"/>
+    <s v="april"/>
+    <x v="1"/>
+    <n v="16835.037999999993"/>
+    <n v="15598.886999999995"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="05"/>
+    <s v="mai"/>
+    <x v="1"/>
+    <n v="17404.65600000001"/>
+    <n v="17502.248999999996"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="06"/>
+    <s v="juni"/>
+    <x v="1"/>
+    <n v="18793.174999999999"/>
+    <n v="19353.077000000005"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="07"/>
+    <s v="juli"/>
+    <x v="1"/>
+    <n v="13163.899999999994"/>
+    <n v="11315.180000000004"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="08"/>
+    <s v="august"/>
+    <x v="1"/>
+    <n v="17447.914999999994"/>
+    <n v="17721.317999999996"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="09"/>
+    <s v="september"/>
+    <x v="1"/>
+    <n v="19644.216999999982"/>
+    <n v="19680.096000000001"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="10"/>
+    <s v="oktober"/>
+    <x v="1"/>
+    <n v="20879.875000000007"/>
+    <n v="19957.396999999997"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="11"/>
+    <s v="november"/>
+    <x v="1"/>
+    <n v="19950.113999999998"/>
+    <n v="19477.366999999991"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="12"/>
+    <s v="desember"/>
+    <x v="1"/>
+    <n v="17818.454000000002"/>
+    <n v="17674.356000000007"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="01"/>
+    <s v="januar"/>
+    <x v="2"/>
+    <n v="19289.946999999996"/>
+    <n v="18698.373999999985"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="02"/>
+    <s v="februar"/>
+    <x v="2"/>
+    <n v="17538.080999999984"/>
+    <n v="16725.26400000001"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="03"/>
+    <s v="mars"/>
+    <x v="2"/>
+    <n v="20321.337"/>
+    <n v="20754.897999999983"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="04"/>
+    <s v="april"/>
+    <x v="2"/>
+    <n v="18171.131999999998"/>
+    <n v="16922.889999999996"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="05"/>
+    <s v="mai"/>
+    <x v="2"/>
+    <n v="18784.802000000011"/>
+    <n v="18729.341000000008"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="06"/>
+    <s v="juni"/>
+    <x v="2"/>
+    <n v="20504.034"/>
+    <n v="18617.498"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="07"/>
+    <s v="juli"/>
+    <x v="2"/>
+    <n v="14146.687999999996"/>
+    <n v="9744.6739999999972"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="08"/>
+    <s v="august"/>
+    <x v="2"/>
+    <n v="18950.996999999999"/>
+    <n v="17095.359000000004"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="09"/>
+    <s v="september"/>
+    <x v="2"/>
+    <n v="23528.81399999998"/>
+    <n v="20555.621999999988"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="10"/>
+    <s v="oktober"/>
+    <x v="2"/>
+    <n v="23380.741999999998"/>
+    <n v="20822.426000000014"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="11"/>
+    <s v="november"/>
+    <x v="2"/>
+    <n v="21902.332999999991"/>
+    <n v="20567.83300000001"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="12"/>
+    <s v="desember"/>
+    <x v="2"/>
+    <n v="19189.556"/>
+    <n v="19570.158000000018"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="01"/>
+    <s v="januar"/>
+    <x v="3"/>
+    <n v="11243.083000000004"/>
+    <n v="11312.26499999999"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="02"/>
+    <s v="februar"/>
+    <x v="3"/>
+    <n v="11064.213999999994"/>
+    <n v="11248.701999999999"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="03"/>
+    <s v="mars"/>
+    <x v="3"/>
+    <n v="13113.727000000003"/>
+    <n v="13500.669999999998"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="04"/>
+    <s v="april"/>
+    <x v="3"/>
+    <n v="15343.574999999997"/>
+    <n v="13265.298999999997"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="05"/>
+    <s v="mai"/>
+    <x v="3"/>
+    <n v="10923.683999999999"/>
+    <n v="12574.346999999998"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="06"/>
+    <s v="juni"/>
+    <x v="3"/>
+    <n v="10285.636000000004"/>
+    <n v="13036.281000000003"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="07"/>
+    <s v="juli"/>
+    <x v="3"/>
+    <n v="5456.6630000000032"/>
+    <n v="7659.3849999999984"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="08"/>
+    <s v="august"/>
+    <x v="3"/>
+    <n v="10049.797000000004"/>
+    <n v="10957.011999999999"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="09"/>
+    <s v="september"/>
+    <x v="3"/>
+    <n v="10668.959000000004"/>
+    <n v="11759.782000000001"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="10"/>
+    <s v="oktober"/>
+    <x v="3"/>
+    <n v="11642.913"/>
+    <n v="13222.791999999999"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="11"/>
+    <s v="november"/>
+    <x v="3"/>
+    <n v="11878.701999999997"/>
+    <n v="12543.041000000008"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="12"/>
+    <s v="desember"/>
+    <x v="3"/>
+    <n v="9898.1810000000023"/>
+    <n v="13046.663000000019"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="01"/>
+    <s v="januar"/>
+    <x v="4"/>
+    <n v="26684.41800000002"/>
+    <n v="26365.247000000018"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="02"/>
+    <s v="februar"/>
+    <x v="4"/>
+    <n v="24267.440999999992"/>
+    <n v="24192.606"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="03"/>
+    <s v="mars"/>
+    <x v="4"/>
+    <n v="29017.515999999996"/>
+    <n v="29248.806000000022"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="04"/>
+    <s v="april"/>
+    <x v="4"/>
+    <n v="25780.440999999999"/>
+    <n v="24608.125999999989"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="05"/>
+    <s v="mai"/>
+    <x v="4"/>
+    <n v="26041.324000000001"/>
+    <n v="26842.398999999998"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="06"/>
+    <s v="juni"/>
+    <x v="4"/>
+    <n v="30151.150999999998"/>
+    <n v="28892.551000000007"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="07"/>
+    <s v="juli"/>
+    <x v="4"/>
+    <n v="15840.230000000009"/>
+    <n v="13820.452000000005"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="08"/>
+    <s v="august"/>
+    <x v="4"/>
+    <n v="27864.148999999987"/>
+    <n v="25675.847000000002"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="09"/>
+    <s v="september"/>
+    <x v="4"/>
+    <n v="30630.966999999997"/>
+    <n v="30294.321000000004"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="10"/>
+    <s v="oktober"/>
+    <x v="4"/>
+    <n v="31183.768999999986"/>
+    <n v="30464.396999999997"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="11"/>
+    <s v="november"/>
+    <x v="4"/>
+    <n v="29438.715999999979"/>
+    <n v="29018.001000000004"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="12"/>
+    <s v="desember"/>
+    <x v="4"/>
+    <n v="27405.461000000018"/>
+    <n v="25251.29599999998"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="01"/>
+    <s v="januar"/>
+    <x v="5"/>
+    <n v="16281.427000000007"/>
+    <n v="14274.425999999998"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="02"/>
+    <s v="februar"/>
+    <x v="5"/>
+    <n v="14463.427000000007"/>
+    <n v="13313.458999999986"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="03"/>
+    <s v="mars"/>
+    <x v="5"/>
+    <n v="16556.241000000002"/>
+    <n v="15102.211000000005"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="04"/>
+    <s v="april"/>
+    <x v="5"/>
+    <n v="15679.055999999999"/>
+    <n v="13007.539999999997"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="05"/>
+    <s v="mai"/>
+    <x v="5"/>
+    <n v="15939.386999999997"/>
+    <n v="14574.513999999999"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="06"/>
+    <s v="juni"/>
+    <x v="5"/>
+    <n v="16164.649000000003"/>
+    <n v="14660.552"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="07"/>
+    <s v="juli"/>
+    <x v="5"/>
+    <n v="12251.258000000002"/>
+    <n v="7782.0099999999975"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="08"/>
+    <s v="august"/>
+    <x v="5"/>
+    <n v="15217.858999999997"/>
+    <n v="14200.076999999996"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="09"/>
+    <s v="september"/>
+    <x v="5"/>
+    <n v="17747.304000000004"/>
+    <n v="14645.768999999997"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="10"/>
+    <s v="oktober"/>
+    <x v="5"/>
+    <n v="18804.403999999995"/>
+    <n v="15894.622000000001"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="11"/>
+    <s v="november"/>
+    <x v="5"/>
+    <n v="17962.565000000028"/>
+    <n v="16089.605000000003"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="12"/>
+    <s v="desember"/>
+    <x v="5"/>
+    <n v="16096.747000000003"/>
+    <n v="15709.048999999994"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="01"/>
+    <s v="januar"/>
+    <x v="6"/>
+    <n v="12632.114000000001"/>
+    <n v="13955.956000000015"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="02"/>
+    <s v="februar"/>
+    <x v="6"/>
+    <n v="11660.077999999998"/>
+    <n v="12605.767000000003"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="03"/>
+    <s v="mars"/>
+    <x v="6"/>
+    <n v="14658.205000000009"/>
+    <n v="15112.570000000002"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="04"/>
+    <s v="april"/>
+    <x v="6"/>
+    <n v="11585.304000000004"/>
+    <n v="13086.752"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="05"/>
+    <s v="mai"/>
+    <x v="6"/>
+    <n v="12642.668999999994"/>
+    <n v="13623.060000000001"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="06"/>
+    <s v="juni"/>
+    <x v="6"/>
+    <n v="12337.938999999998"/>
+    <n v="13592.904"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="07"/>
+    <s v="juli"/>
+    <x v="6"/>
+    <n v="5870.7689999999993"/>
+    <n v="7441.1400000000049"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="08"/>
+    <s v="august"/>
+    <x v="6"/>
+    <n v="11252.06"/>
+    <n v="13434.850999999999"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="09"/>
+    <s v="september"/>
+    <x v="6"/>
+    <n v="12975.283000000001"/>
+    <n v="15266.221000000001"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="10"/>
+    <s v="oktober"/>
+    <x v="6"/>
+    <n v="13241.894000000008"/>
+    <n v="15040.923999999995"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="11"/>
+    <s v="november"/>
+    <x v="6"/>
+    <n v="13169.750999999997"/>
+    <n v="14640.900000000007"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="12"/>
+    <s v="desember"/>
+    <x v="6"/>
+    <n v="11754.716999999995"/>
+    <n v="11925.112999999994"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="01"/>
+    <s v="januar"/>
+    <x v="7"/>
+    <n v="7690.1029999999982"/>
+    <n v="6842.3710000000019"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="02"/>
+    <s v="februar"/>
+    <x v="7"/>
+    <n v="6807.2900000000027"/>
+    <n v="6623.6380000000026"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="03"/>
+    <s v="mars"/>
+    <x v="7"/>
+    <n v="8450.3539999999975"/>
+    <n v="8494.4139999999952"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="04"/>
+    <s v="april"/>
+    <x v="7"/>
+    <n v="7342.4800000000032"/>
+    <n v="7146.6990000000005"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="05"/>
+    <s v="mai"/>
+    <x v="7"/>
+    <n v="7920.9680000000026"/>
+    <n v="7657.6549999999997"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="06"/>
+    <s v="juni"/>
+    <x v="7"/>
+    <n v="10329.530999999999"/>
+    <n v="9189.0529999999999"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="07"/>
+    <s v="juli"/>
+    <x v="7"/>
+    <n v="17641.983000000007"/>
+    <n v="13466.424000000005"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="08"/>
+    <s v="august"/>
+    <x v="7"/>
+    <n v="10746.399000000001"/>
+    <n v="9924.5400000000045"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="09"/>
+    <s v="september"/>
+    <x v="7"/>
+    <n v="8700.8799999999901"/>
+    <n v="8339.7940000000071"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="10"/>
+    <s v="oktober"/>
+    <x v="7"/>
+    <n v="8651.8349999999991"/>
+    <n v="8594.0320000000011"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="11"/>
+    <s v="november"/>
+    <x v="7"/>
+    <n v="8451.1270000000004"/>
+    <n v="8242.5300000000007"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="12"/>
+    <s v="desember"/>
+    <x v="7"/>
+    <n v="7727.9400000000023"/>
+    <n v="6662.3369999999977"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="01"/>
+    <s v="januar"/>
+    <x v="8"/>
+    <n v="10026.708999999992"/>
+    <n v="9407.6890000000021"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="02"/>
+    <s v="februar"/>
+    <x v="8"/>
+    <n v="8609.9560000000019"/>
+    <n v="8810.0460000000003"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="03"/>
+    <s v="mars"/>
+    <x v="8"/>
+    <n v="9624.2999999999956"/>
+    <n v="10125.351999999997"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="04"/>
+    <s v="april"/>
+    <x v="8"/>
+    <n v="10734.928000000002"/>
+    <n v="8433.0500000000011"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="05"/>
+    <s v="mai"/>
+    <x v="8"/>
+    <n v="10117.042999999994"/>
+    <n v="9168.8320000000003"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="06"/>
+    <s v="juni"/>
+    <x v="8"/>
+    <n v="10121.277000000002"/>
+    <n v="10484.320999999996"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="07"/>
+    <s v="juli"/>
+    <x v="8"/>
+    <n v="6620.431000000005"/>
+    <n v="5812.9209999999985"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="08"/>
+    <s v="august"/>
+    <x v="8"/>
+    <n v="10778.187000000002"/>
+    <n v="10453.581999999999"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="09"/>
+    <s v="september"/>
+    <x v="8"/>
+    <n v="9809.051999999996"/>
+    <n v="10965.622999999992"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="10"/>
+    <s v="oktober"/>
+    <x v="8"/>
+    <n v="10092.341000000004"/>
+    <n v="9465.5349999999962"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="11"/>
+    <s v="november"/>
+    <x v="8"/>
+    <n v="9627.9109999999982"/>
+    <n v="8712.0240000000013"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="12"/>
+    <s v="desember"/>
+    <x v="8"/>
+    <n v="7977.3580000000111"/>
+    <n v="8905.546999999995"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="01"/>
+    <s v="januar"/>
+    <x v="9"/>
+    <n v="52569.733000000007"/>
+    <n v="52550.710000000057"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="02"/>
+    <s v="februar"/>
+    <x v="9"/>
+    <n v="47709.025999999998"/>
+    <n v="47559.052999999971"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="03"/>
+    <s v="mars"/>
+    <x v="9"/>
+    <n v="56888.356000000043"/>
+    <n v="56953.466999999997"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="04"/>
+    <s v="april"/>
+    <x v="9"/>
+    <n v="48054.907999999981"/>
+    <n v="47166.648999999998"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="05"/>
+    <s v="mai"/>
+    <x v="9"/>
+    <n v="51552.485000000022"/>
+    <n v="52605.115000000049"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="06"/>
+    <s v="juni"/>
+    <x v="9"/>
+    <n v="52139.282000000007"/>
+    <n v="51498.349999999991"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="07"/>
+    <s v="juli"/>
+    <x v="9"/>
+    <n v="32373.516000000018"/>
+    <n v="24574.998000000018"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="08"/>
+    <s v="august"/>
+    <x v="9"/>
+    <n v="49687.463000000003"/>
+    <n v="48314.031999999977"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="09"/>
+    <s v="september"/>
+    <x v="9"/>
+    <n v="53142.930000000008"/>
+    <n v="54783.914999999979"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="10"/>
+    <s v="oktober"/>
+    <x v="9"/>
+    <n v="54904.841000000059"/>
+    <n v="55629.769000000044"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="11"/>
+    <s v="november"/>
+    <x v="9"/>
+    <n v="54830.934000000001"/>
+    <n v="55156.104999999981"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="12"/>
+    <s v="desember"/>
+    <x v="9"/>
+    <n v="47248.511000000079"/>
+    <n v="49729.573000000048"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="01"/>
+    <s v="januar"/>
+    <x v="10"/>
+    <n v="13390.534999999987"/>
+    <n v="14996.275999999994"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="01"/>
+    <s v="januar"/>
+    <x v="11"/>
+    <n v="15138.191999999992"/>
+    <n v="14145.188000000002"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="01"/>
+    <s v="januar"/>
+    <x v="12"/>
+    <n v="18196.075000000012"/>
+    <n v="16920.315000000002"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="01"/>
+    <s v="januar"/>
+    <x v="13"/>
+    <n v="8758.7370000000064"/>
+    <n v="11545.432000000004"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="01"/>
+    <s v="januar"/>
+    <x v="14"/>
+    <n v="23042.861999999983"/>
+    <n v="20762.964000000011"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="01"/>
+    <s v="januar"/>
+    <x v="15"/>
+    <n v="14904.721000000003"/>
+    <n v="11821.954999999996"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="01"/>
+    <s v="januar"/>
+    <x v="16"/>
+    <n v="9706.2029999999941"/>
+    <n v="10967.348000000007"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="01"/>
+    <s v="januar"/>
+    <x v="17"/>
+    <n v="6110.3560000000025"/>
+    <n v="5183.4159999999956"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="01"/>
+    <s v="januar"/>
+    <x v="18"/>
+    <n v="38691.027000000038"/>
+    <n v="40533.070999999924"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="01"/>
+    <s v="januar"/>
+    <x v="19"/>
+    <n v="8289.2579999999907"/>
+    <n v="7765.6389999999974"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="02"/>
+    <s v="februar"/>
+    <x v="10"/>
+    <n v="13514.843000000008"/>
+    <n v="16473.749000000011"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="02"/>
+    <s v="februar"/>
+    <x v="11"/>
+    <n v="15382.436000000007"/>
+    <n v="14463.429"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="02"/>
+    <s v="februar"/>
+    <x v="12"/>
+    <n v="18223.679000000004"/>
+    <n v="18131.571999999993"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="02"/>
+    <s v="februar"/>
+    <x v="13"/>
+    <n v="8614.3990000000031"/>
+    <n v="13155.784000000007"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="02"/>
+    <s v="februar"/>
+    <x v="14"/>
+    <n v="24535.053"/>
+    <n v="21851.250000000015"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="02"/>
+    <s v="februar"/>
+    <x v="15"/>
+    <n v="14959.259999999987"/>
+    <n v="13582.722000000002"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="02"/>
+    <s v="februar"/>
+    <x v="16"/>
+    <n v="10196.832999999995"/>
+    <n v="11076.638000000006"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="02"/>
+    <s v="februar"/>
+    <x v="17"/>
+    <n v="7111.2660000000024"/>
+    <n v="6014.4710000000023"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="02"/>
+    <s v="februar"/>
+    <x v="18"/>
+    <n v="39863.910000000003"/>
+    <n v="43578.042999999983"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="02"/>
+    <s v="februar"/>
+    <x v="19"/>
+    <n v="8554.992000000002"/>
+    <n v="7979.3529999999964"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="03"/>
+    <s v="mars"/>
+    <x v="10"/>
+    <n v="14554.614000000016"/>
+    <n v="17767.417999999998"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="03"/>
+    <s v="mars"/>
+    <x v="11"/>
+    <n v="16230.686000000016"/>
+    <n v="14217.76300000001"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="03"/>
+    <s v="mars"/>
+    <x v="12"/>
+    <n v="19148.013999999999"/>
+    <n v="18437.450000000008"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="03"/>
+    <s v="mars"/>
+    <x v="13"/>
+    <n v="9875.8120000000072"/>
+    <n v="14581.028999999999"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="03"/>
+    <s v="mars"/>
+    <x v="14"/>
+    <n v="24331.954000000005"/>
+    <n v="21516.736999999979"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="03"/>
+    <s v="mars"/>
+    <x v="15"/>
+    <n v="15937.729999999996"/>
+    <n v="13662.458999999999"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="03"/>
+    <s v="mars"/>
+    <x v="16"/>
+    <n v="11562.04999999999"/>
+    <n v="12496.948000000008"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="03"/>
+    <s v="mars"/>
+    <x v="17"/>
+    <n v="7938.7159999999967"/>
+    <n v="6567.2850000000044"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="03"/>
+    <s v="mars"/>
+    <x v="18"/>
+    <n v="40197.795999999995"/>
+    <n v="49090.64799999995"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="03"/>
+    <s v="mars"/>
+    <x v="19"/>
+    <n v="8672.8129999999983"/>
+    <n v="8418.6619999999948"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="04"/>
+    <s v="april"/>
+    <x v="10"/>
+    <n v="15086.74800000002"/>
+    <n v="17013.539000000004"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="04"/>
+    <s v="april"/>
+    <x v="11"/>
+    <n v="16820.261000000024"/>
+    <n v="15605.163999999986"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="04"/>
+    <s v="april"/>
+    <x v="12"/>
+    <n v="20968.641000000003"/>
+    <n v="19727.482999999993"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="04"/>
+    <s v="april"/>
+    <x v="13"/>
+    <n v="10286.784999999994"/>
+    <n v="13921.527999999995"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="04"/>
+    <s v="april"/>
+    <x v="14"/>
+    <n v="27443.664000000048"/>
+    <n v="24818.852999999988"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="04"/>
+    <s v="april"/>
+    <x v="15"/>
+    <n v="16300.301000000003"/>
+    <n v="14012.694000000007"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="04"/>
+    <s v="april"/>
+    <x v="16"/>
+    <n v="11533.723000000002"/>
+    <n v="11803.738999999994"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="04"/>
+    <s v="april"/>
+    <x v="17"/>
+    <n v="7470.2369999999928"/>
+    <n v="5711.5980000000018"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="04"/>
+    <s v="april"/>
+    <x v="18"/>
+    <n v="42898.463999999978"/>
+    <n v="45229.885000000017"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="04"/>
+    <s v="april"/>
+    <x v="19"/>
+    <n v="9156.1990000000005"/>
+    <n v="8813.0069999999978"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <m/>
+    <m/>
+    <x v="20"/>
+    <m/>
+    <m/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6543A394-9255-4FFA-9DDF-53C434B76B04}" name="Pivottabell1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Verdier" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:N7" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="4">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="12">
+        <item h="1" x="0"/>
+        <item h="1" x="1"/>
+        <item x="2"/>
+        <item h="1" x="3"/>
+        <item h="1" x="4"/>
+        <item x="5"/>
+        <item h="1" x="6"/>
+        <item h="1" x="7"/>
+        <item h="1" x="8"/>
+        <item h="1" x="9"/>
+        <item h="1" x="10"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="14">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="3"/>
+  </colFields>
+  <colItems count="13">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Summer av Antall_av_på" fld="2" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2E93EAE1-8E0E-4B8E-B7C5-19716A7F6A94}" name="Pivottabell2" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Verdier" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:G10" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
+  <pivotFields count="6">
+    <pivotField axis="axisCol" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="22">
+        <item h="1" x="0"/>
+        <item h="1" x="10"/>
+        <item h="1" x="1"/>
+        <item h="1" x="11"/>
+        <item x="2"/>
+        <item x="12"/>
+        <item h="1" x="3"/>
+        <item h="1" x="13"/>
+        <item h="1" x="4"/>
+        <item h="1" x="14"/>
+        <item x="5"/>
+        <item x="15"/>
+        <item h="1" x="6"/>
+        <item h="1" x="16"/>
+        <item h="1" x="7"/>
+        <item h="1" x="17"/>
+        <item h="1" x="8"/>
+        <item h="1" x="19"/>
+        <item h="1" x="9"/>
+        <item h="1" x="18"/>
+        <item h="1" x="20"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="2">
+    <field x="0"/>
+    <field x="-2"/>
+  </colFields>
+  <colItems count="6">
+    <i>
+      <x/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="1"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Summer av Påstigninger" fld="4" baseField="0" baseItem="0"/>
+    <dataField name="Summer av Avstigninger" fld="5" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-tema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013–2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -502,7 +2894,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013–2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -608,7 +3000,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013–2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -750,18 +3142,224 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC104E46-1C33-402B-A683-BE30745DCD6A}">
+  <dimension ref="A3:N7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="13" width="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4">
+        <v>2012</v>
+      </c>
+      <c r="C4">
+        <v>2013</v>
+      </c>
+      <c r="D4">
+        <v>2014</v>
+      </c>
+      <c r="E4">
+        <v>2015</v>
+      </c>
+      <c r="F4">
+        <v>2016</v>
+      </c>
+      <c r="G4">
+        <v>2017</v>
+      </c>
+      <c r="H4">
+        <v>2018</v>
+      </c>
+      <c r="I4">
+        <v>2019</v>
+      </c>
+      <c r="J4">
+        <v>2020</v>
+      </c>
+      <c r="K4">
+        <v>2021</v>
+      </c>
+      <c r="L4">
+        <v>2022</v>
+      </c>
+      <c r="M4">
+        <v>2023</v>
+      </c>
+      <c r="N4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="18">
+        <v>141379</v>
+      </c>
+      <c r="C5" s="18">
+        <v>190114</v>
+      </c>
+      <c r="D5" s="18">
+        <v>198514</v>
+      </c>
+      <c r="E5" s="18">
+        <v>217635</v>
+      </c>
+      <c r="F5" s="18">
+        <v>268098</v>
+      </c>
+      <c r="G5" s="18">
+        <v>95402</v>
+      </c>
+      <c r="H5" s="18">
+        <v>115993</v>
+      </c>
+      <c r="I5" s="18">
+        <v>291603</v>
+      </c>
+      <c r="J5" s="18">
+        <v>179134</v>
+      </c>
+      <c r="K5" s="18">
+        <v>151838</v>
+      </c>
+      <c r="L5" s="18">
+        <v>300022</v>
+      </c>
+      <c r="M5" s="18">
+        <v>454512</v>
+      </c>
+      <c r="N5" s="18">
+        <v>2604244</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="18">
+        <v>80101</v>
+      </c>
+      <c r="C6" s="18">
+        <v>112886</v>
+      </c>
+      <c r="D6" s="18">
+        <v>119997</v>
+      </c>
+      <c r="E6" s="18">
+        <v>126139</v>
+      </c>
+      <c r="F6" s="18">
+        <v>145151</v>
+      </c>
+      <c r="G6" s="18">
+        <v>77829</v>
+      </c>
+      <c r="H6" s="18">
+        <v>97152</v>
+      </c>
+      <c r="I6" s="18">
+        <v>220938</v>
+      </c>
+      <c r="J6" s="18">
+        <v>151023</v>
+      </c>
+      <c r="K6" s="18">
+        <v>127373</v>
+      </c>
+      <c r="L6" s="18">
+        <v>207067</v>
+      </c>
+      <c r="M6" s="18">
+        <v>362417</v>
+      </c>
+      <c r="N6" s="18">
+        <v>1828073</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" s="18">
+        <v>221480</v>
+      </c>
+      <c r="C7" s="18">
+        <v>303000</v>
+      </c>
+      <c r="D7" s="18">
+        <v>318511</v>
+      </c>
+      <c r="E7" s="18">
+        <v>343774</v>
+      </c>
+      <c r="F7" s="18">
+        <v>413249</v>
+      </c>
+      <c r="G7" s="18">
+        <v>173231</v>
+      </c>
+      <c r="H7" s="18">
+        <v>213145</v>
+      </c>
+      <c r="I7" s="18">
+        <v>512541</v>
+      </c>
+      <c r="J7" s="18">
+        <v>330157</v>
+      </c>
+      <c r="K7" s="18">
+        <v>279211</v>
+      </c>
+      <c r="L7" s="18">
+        <v>507089</v>
+      </c>
+      <c r="M7" s="18">
+        <v>816929</v>
+      </c>
+      <c r="N7" s="18">
+        <v>4432317</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25D0B74A-329A-43D4-ACFD-DCC824F63451}">
   <dimension ref="A1:N121"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2577,17 +5175,198 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E121" xr:uid="{25D0B74A-329A-43D4-ACFD-DCC824F63451}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6A705A9-E048-4296-8614-3B3CCC204092}">
+  <dimension ref="A3:G13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:G9"/>
+      <pivotSelection pane="bottomRight" showHeader="1" extendable="1" axis="axisRow" start="3" max="5" activeRow="8" previousRow="8" click="1" r:id="rId1">
+        <pivotArea dataOnly="0" fieldPosition="0">
+          <references count="1">
+            <reference field="3" count="1">
+              <x v="11"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotSelection>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B3" s="16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>2023</v>
+      </c>
+      <c r="D4">
+        <v>2024</v>
+      </c>
+      <c r="F4" t="s">
+        <v>75</v>
+      </c>
+      <c r="G4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="18">
+        <v>235708.46299999999</v>
+      </c>
+      <c r="C6" s="18">
+        <v>218804.33699999997</v>
+      </c>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18">
+        <v>235708.46299999999</v>
+      </c>
+      <c r="G6" s="18">
+        <v>218804.33699999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18">
+        <v>76536.409000000014</v>
+      </c>
+      <c r="E7" s="18">
+        <v>73216.820000000007</v>
+      </c>
+      <c r="F7" s="18">
+        <v>76536.409000000014</v>
+      </c>
+      <c r="G7" s="18">
+        <v>73216.820000000007</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="18">
+        <v>193164.32400000005</v>
+      </c>
+      <c r="C8" s="18">
+        <v>169253.83399999994</v>
+      </c>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18">
+        <v>193164.32400000005</v>
+      </c>
+      <c r="G8" s="18">
+        <v>169253.83399999994</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18">
+        <v>62102.011999999988</v>
+      </c>
+      <c r="E9" s="18">
+        <v>53079.83</v>
+      </c>
+      <c r="F9" s="18">
+        <v>62102.011999999988</v>
+      </c>
+      <c r="G9" s="18">
+        <v>53079.83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" s="18">
+        <v>428872.78700000001</v>
+      </c>
+      <c r="C10" s="18">
+        <v>388058.17099999991</v>
+      </c>
+      <c r="D10" s="18">
+        <v>138638.421</v>
+      </c>
+      <c r="E10" s="18">
+        <v>126296.65000000001</v>
+      </c>
+      <c r="F10" s="18">
+        <v>567511.20799999998</v>
+      </c>
+      <c r="G10" s="18">
+        <v>514354.82099999994</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <f>SUM(B6:C9)</f>
+        <v>816930.95799999987</v>
+      </c>
+      <c r="D13">
+        <f>SUM(D6:E9)</f>
+        <v>264935.071</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DE9A58E-6281-4D08-BF08-9517A14C48DB}">
   <dimension ref="A1:J161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
-      <selection activeCell="J134" sqref="J134"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6717,7 +9496,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BAE721D-EEC0-4576-A3CE-F52737DC4230}">
   <dimension ref="A1:E2"/>
   <sheetViews>

</xml_diff>